<commit_message>
Mejoras de diseño, cambios de funcionalidad
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imail\OneDrive\Desktop\CODIGO ESTADIAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/904702f6d0479124/Desktop/CODIGO ESTADIAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A943CC1C-6024-4EB1-A8DD-B7FACAF5FF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A943CC1C-6024-4EB1-A8DD-B7FACAF5FF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CC453CF-1ACB-473B-8AB3-C8E4E19F1A11}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{565769C0-9636-4B43-A96D-04180A898660}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{565769C0-9636-4B43-A96D-04180A898660}"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>PIEZAS</t>
   </si>
@@ -51,6 +50,9 @@
   </si>
   <si>
     <t>Gatito</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
   </si>
 </sst>
 </file>
@@ -402,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6E5EDA-C5B2-4548-AFD8-FF26EB1D47AC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,18 +415,21 @@
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="D1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -434,8 +439,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -443,6 +451,9 @@
         <v>1213487942</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
     </row>
@@ -455,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEF0E94-78CD-4130-839E-FAA995363619}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>

</xml_diff>